<commit_message>
excel update & login request update
</commit_message>
<xml_diff>
--- a/Project Apis.xlsx
+++ b/Project Apis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\UK\QuoraStudent\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\project\QuoraStudent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A34F71-7AF1-4404-8CED-E8CA55D47A12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F3F7CE-2E44-4C03-93E7-E42768BE8FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Apis" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
   <si>
     <t xml:space="preserve">params </t>
   </si>
@@ -161,6 +161,18 @@
   </si>
   <si>
     <t>{userid: xxx, interests: [ {id:34,name: '' }]  }</t>
+  </si>
+  <si>
+    <t>5th-6th July</t>
+  </si>
+  <si>
+    <t>user/askQuestion</t>
+  </si>
+  <si>
+    <t>{data:{updated},sucsess:true,reason:null}</t>
+  </si>
+  <si>
+    <t>{userid:xxx,text:xxx,tags:[id1,id2,]}</t>
   </si>
 </sst>
 </file>
@@ -208,7 +220,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -231,11 +243,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -254,6 +277,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -276,15 +300,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>426721</xdr:colOff>
+      <xdr:colOff>248921</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>388621</xdr:rowOff>
+      <xdr:rowOff>280671</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2567940</xdr:colOff>
+      <xdr:colOff>2390140</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>1796995</xdr:rowOff>
+      <xdr:rowOff>1689045</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -313,7 +337,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1036321" y="2948941"/>
+          <a:off x="858521" y="2858771"/>
           <a:ext cx="2141219" cy="1408374"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -365,6 +389,56 @@
         <a:xfrm>
           <a:off x="1181100" y="5516880"/>
           <a:ext cx="1577340" cy="1183005"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>154214</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2748643</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>2131786</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37D0948D-7519-4105-80A0-FF3E05C977BD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="874486" y="6622143"/>
+          <a:ext cx="2481943" cy="1977572"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -641,22 +715,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="42.77734375" customWidth="1"/>
-    <col min="3" max="3" width="43.6640625" customWidth="1"/>
-    <col min="4" max="4" width="30.109375" customWidth="1"/>
+    <col min="2" max="2" width="42.81640625" customWidth="1"/>
+    <col min="3" max="3" width="43.6328125" customWidth="1"/>
+    <col min="4" max="4" width="30.08984375" customWidth="1"/>
     <col min="5" max="5" width="42" customWidth="1"/>
-    <col min="6" max="6" width="31.33203125" customWidth="1"/>
-    <col min="7" max="7" width="24.109375" customWidth="1"/>
-    <col min="8" max="8" width="57.88671875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="31.36328125" customWidth="1"/>
+    <col min="7" max="7" width="24.08984375" customWidth="1"/>
+    <col min="8" max="8" width="57.90625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -670,12 +744,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -689,7 +763,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -703,7 +777,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -717,7 +791,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>9</v>
       </c>
@@ -731,12 +805,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B8" s="11" t="s">
         <v>14</v>
       </c>
@@ -747,12 +821,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B10" s="6" t="s">
         <v>33</v>
       </c>
@@ -766,7 +840,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B11" s="6" t="s">
         <v>34</v>
       </c>
@@ -780,7 +854,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B13" s="4" t="s">
         <v>21</v>
       </c>
@@ -791,7 +865,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>26</v>
       </c>
@@ -817,7 +891,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="151.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="151.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>1</v>
       </c>
@@ -833,7 +907,7 @@
       <c r="G15" s="3"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" ht="129.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="129.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>2</v>
       </c>
@@ -855,7 +929,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -873,8 +947,26 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="185.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
+      <c r="C18" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -891,32 +983,32 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
Ask a question changes
</commit_message>
<xml_diff>
--- a/Project Apis.xlsx
+++ b/Project Apis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\project\QuoraStudent\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\UK\QuoraStudent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F3F7CE-2E44-4C03-93E7-E42768BE8FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E004EEAB-9082-4F0A-9EF8-998E549D806C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Apis" sheetId="1" r:id="rId1"/>
@@ -166,13 +166,21 @@
     <t>5th-6th July</t>
   </si>
   <si>
-    <t>user/askQuestion</t>
-  </si>
-  <si>
-    <t>{data:{updated},sucsess:true,reason:null}</t>
-  </si>
-  <si>
-    <t>{userid:xxx,text:xxx,tags:[id1,id2,]}</t>
+    <t>/questions/askAquestion</t>
+  </si>
+  <si>
+    <t>{
+    "userid":6,"text":"&lt;h1&gt;How do the college manage marks&lt;/h1&gt; ","tags":[1,2,3]
+}</t>
+  </si>
+  <si>
+    <t>{
+    "data": {
+        "updated": true
+    },
+    "success": true,
+    "reason": null
+}</t>
   </si>
 </sst>
 </file>
@@ -715,22 +723,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="42.81640625" customWidth="1"/>
-    <col min="3" max="3" width="43.6328125" customWidth="1"/>
-    <col min="4" max="4" width="30.08984375" customWidth="1"/>
+    <col min="2" max="2" width="42.77734375" customWidth="1"/>
+    <col min="3" max="3" width="43.6640625" customWidth="1"/>
+    <col min="4" max="4" width="30.109375" customWidth="1"/>
     <col min="5" max="5" width="42" customWidth="1"/>
-    <col min="6" max="6" width="31.36328125" customWidth="1"/>
-    <col min="7" max="7" width="24.08984375" customWidth="1"/>
-    <col min="8" max="8" width="57.90625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="31.33203125" customWidth="1"/>
+    <col min="7" max="7" width="24.109375" customWidth="1"/>
+    <col min="8" max="8" width="57.88671875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -744,12 +752,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -763,7 +771,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -777,7 +785,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -791,7 +799,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>9</v>
       </c>
@@ -805,12 +813,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8" s="11" t="s">
         <v>14</v>
       </c>
@@ -821,12 +829,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
         <v>33</v>
       </c>
@@ -840,7 +848,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
         <v>34</v>
       </c>
@@ -854,7 +862,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" s="4" t="s">
         <v>21</v>
       </c>
@@ -865,7 +873,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>26</v>
       </c>
@@ -891,7 +899,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="151.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="151.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
@@ -907,7 +915,7 @@
       <c r="G15" s="3"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" ht="129.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="129.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>2</v>
       </c>
@@ -929,7 +937,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -947,7 +955,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="185.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="185.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="C18" s="12" t="s">
         <v>45</v>
@@ -958,14 +966,14 @@
       <c r="E18" t="s">
         <v>46</v>
       </c>
-      <c r="F18" t="s">
-        <v>48</v>
+      <c r="F18" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="G18" s="12" t="s">
         <v>6</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -983,32 +991,32 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>41</v>
       </c>

</xml_diff>